<commit_message>
Updated test data of carry bag with new store, user id's
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/carry_bag_test_data.xlsx
+++ b/TestData/Web_POS/Billing/carry_bag_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="199" count="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="210" count="378">
   <si>
     <t>TC_Id</t>
   </si>
@@ -611,6 +611,39 @@
   </si>
   <si>
     <t>CB_16</t>
+  </si>
+  <si>
+    <t>userone_p1</t>
+  </si>
+  <si>
+    <t>307260624P3E</t>
+  </si>
+  <si>
+    <t>Carry Bag Latest : 1</t>
+  </si>
+  <si>
+    <t>Carry Bag Latest : 2.5</t>
+  </si>
+  <si>
+    <t>Carry Bag Latest : -3</t>
+  </si>
+  <si>
+    <t>Carry Bag Latest : 1, CarryBagNegative : 2</t>
+  </si>
+  <si>
+    <t>Carry Bag Latest : 2</t>
+  </si>
+  <si>
+    <t>cnegative : 1</t>
+  </si>
+  <si>
+    <t>userone_p2</t>
+  </si>
+  <si>
+    <t>307260624ut0</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -691,7 +724,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -711,13 +751,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
@@ -748,6 +788,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,7 +1003,7 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView topLeftCell="L45" view="normal" tabSelected="1" workbookViewId="0">
       <selection pane="topLeft" activeCell="R66" sqref="R66"/>
@@ -1055,7 +1096,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1064,7 +1105,7 @@
         <v>123456</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F2" s="2">
         <v>123456</v>
@@ -1088,7 +1129,7 @@
         <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>172</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>25</v>
@@ -1117,7 +1158,7 @@
         <v>174</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1126,7 +1167,7 @@
         <v>123456</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F3" s="2">
         <v>123456</v>
@@ -1168,7 +1209,7 @@
         <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="T3" t="s">
         <v>25</v>
@@ -1179,7 +1220,7 @@
         <v>177</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -1188,7 +1229,7 @@
         <v>123456</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F4" s="2">
         <v>123456</v>
@@ -1230,7 +1271,7 @@
         <v>25</v>
       </c>
       <c r="S4" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="T4" t="s">
         <v>25</v>
@@ -1241,7 +1282,7 @@
         <v>179</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
@@ -1250,7 +1291,7 @@
         <v>123456</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F5" s="2">
         <v>123456</v>
@@ -1292,7 +1333,7 @@
         <v>25</v>
       </c>
       <c r="S5" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="T5" t="s">
         <v>25</v>
@@ -1303,7 +1344,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
@@ -1312,7 +1353,7 @@
         <v>123456</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F6" s="2">
         <v>123456</v>
@@ -1365,7 +1406,7 @@
         <v>182</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
@@ -1374,7 +1415,7 @@
         <v>123456</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F7" s="2">
         <v>123456</v>
@@ -1416,7 +1457,7 @@
         <v>25</v>
       </c>
       <c r="S7" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="T7" t="s">
         <v>25</v>
@@ -1427,7 +1468,7 @@
         <v>183</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
@@ -1436,7 +1477,7 @@
         <v>123456</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F8" s="2">
         <v>123456</v>
@@ -1478,7 +1519,7 @@
         <v>25</v>
       </c>
       <c r="S8" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="T8" t="s">
         <v>25</v>
@@ -1489,7 +1530,7 @@
         <v>185</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
@@ -1498,7 +1539,7 @@
         <v>123456</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F9" s="2">
         <v>123456</v>
@@ -1540,7 +1581,7 @@
         <v>25</v>
       </c>
       <c r="S9" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="T9" t="s">
         <v>25</v>
@@ -1550,8 +1591,8 @@
       <c r="A10" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>164</v>
+      <c r="B10" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
@@ -1559,8 +1600,8 @@
       <c r="D10" s="2">
         <v>123456</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
+      <c r="E10" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="F10" s="2">
         <v>123456</v>
@@ -1583,8 +1624,8 @@
       <c r="L10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>189</v>
+      <c r="M10" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>25</v>
@@ -1613,7 +1654,7 @@
         <v>190</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
@@ -1622,7 +1663,7 @@
         <v>123456</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F11" s="2">
         <v>123456</v>
@@ -1645,8 +1686,8 @@
       <c r="L11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>189</v>
+      <c r="M11" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>25</v>
@@ -1675,7 +1716,7 @@
         <v>191</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>20</v>
@@ -1684,7 +1725,7 @@
         <v>123456</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F12" s="2">
         <v>123456</v>
@@ -1726,7 +1767,7 @@
         <v>25</v>
       </c>
       <c r="S12" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="T12" t="s">
         <v>25</v>
@@ -1737,7 +1778,7 @@
         <v>192</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
@@ -1746,7 +1787,7 @@
         <v>123456</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F13" s="2">
         <v>123456</v>
@@ -1788,7 +1829,7 @@
         <v>25</v>
       </c>
       <c r="S13" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="T13" t="s">
         <v>25</v>
@@ -1799,7 +1840,7 @@
         <v>193</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
@@ -1808,7 +1849,7 @@
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
@@ -1850,18 +1891,18 @@
         <v>25</v>
       </c>
       <c r="S14" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="T14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="24">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>195</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1870,7 +1911,7 @@
         <v>123456</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F15" s="2">
         <v>123456</v>
@@ -1894,7 +1935,7 @@
         <v>25</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>25</v>
@@ -1918,12 +1959,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="24">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>164</v>
+      <c r="B16" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>20</v>
@@ -1931,8 +1972,8 @@
       <c r="D16" s="2">
         <v>123456</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>21</v>
+      <c r="E16" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="F16" s="2">
         <v>123456</v>
@@ -1956,7 +1997,7 @@
         <v>25</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>25</v>
@@ -1980,12 +2021,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="24">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>198</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>20</v>
@@ -1994,7 +2035,7 @@
         <v>123456</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="F17" s="2">
         <v>123456</v>
@@ -2018,7 +2059,7 @@
         <v>25</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>25</v>
@@ -2052,6 +2093,7 @@
       <c r="T20"/>
     </row>
     <row r="23"/>
+    <row r="24"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>

</xml_diff>

<commit_message>
Tags and Wait Updated
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/carry_bag_test_data.xlsx
+++ b/TestData/Web_POS/Billing/carry_bag_test_data.xlsx
@@ -1,202 +1,224 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Web_POS\Billing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>TC_Id</t>
-  </si>
-  <si>
-    <t>serial_key</t>
-  </si>
-  <si>
-    <t>username_admin</t>
-  </si>
-  <si>
-    <t>password_admin</t>
-  </si>
-  <si>
-    <t>username_pos</t>
-  </si>
-  <si>
-    <t>password_pos</t>
-  </si>
-  <si>
-    <t>closing_balance</t>
-  </si>
-  <si>
-    <t>opening_balance</t>
-  </si>
-  <si>
-    <t>store_name</t>
-  </si>
-  <si>
-    <t>promo_name</t>
-  </si>
-  <si>
-    <t>assortment</t>
-  </si>
-  <si>
-    <t>categories</t>
-  </si>
-  <si>
-    <t>buy_items</t>
-  </si>
-  <si>
-    <t>get_items</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>carry_bag</t>
-  </si>
-  <si>
-    <t>Price_Override</t>
-  </si>
-  <si>
-    <t>tax_invoice</t>
-  </si>
-  <si>
-    <t>CB_1</t>
-  </si>
-  <si>
-    <t>307260624P3E</t>
-  </si>
-  <si>
-    <t>zwshashank.agrawal@teampureplay.com</t>
-  </si>
-  <si>
-    <t>userone_p1</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>CB_2</t>
-  </si>
-  <si>
-    <t>Carry Bag Latest : 1</t>
-  </si>
-  <si>
-    <t>CB_3</t>
-  </si>
-  <si>
-    <t>Carry Bag Latest : 2.5</t>
-  </si>
-  <si>
-    <t>CB_4</t>
-  </si>
-  <si>
-    <t>Carry Bag Latest : -3</t>
-  </si>
-  <si>
-    <t>CB_5</t>
-  </si>
-  <si>
-    <t>CB_6</t>
-  </si>
-  <si>
-    <t>CB_7</t>
-  </si>
-  <si>
-    <t>CB_8</t>
-  </si>
-  <si>
-    <t>Carry Bag Latest : 1, CarryBagNegative : 2</t>
-  </si>
-  <si>
-    <t>CB_9</t>
-  </si>
-  <si>
-    <t>307260624ut0</t>
-  </si>
-  <si>
-    <t>userone_p2</t>
-  </si>
-  <si>
-    <t>8906118412556 : 1</t>
-  </si>
-  <si>
-    <t>CB_10</t>
-  </si>
-  <si>
-    <t>CB_11</t>
-  </si>
-  <si>
-    <t>CB_12</t>
-  </si>
-  <si>
-    <t>CB_13</t>
-  </si>
-  <si>
-    <t>Carry Bag Latest : 2</t>
-  </si>
-  <si>
-    <t>CB_14</t>
-  </si>
-  <si>
-    <t>cnegative : 1</t>
-  </si>
-  <si>
-    <t>CB_15</t>
-  </si>
-  <si>
-    <t>CB_16</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="50">
+  <si>
+    <t xml:space="preserve">TC_Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serial_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username_pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password_pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closing_balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opening_balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promo_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assortment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buy_items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carry_bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price_Override</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624P3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry Bag Latest : 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry Bag Latest : 2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry Bag Latest : -3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry Bag Latest : 1, CarryBagNegative : 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624ut0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8906118412556 : 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry Bag Latest : 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnegative : 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB_16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF2B579A"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF2B579A"/>
-      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,160 +226,258 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E7E7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7E7E7"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFE7E7E7"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="medium">
         <color rgb="FF2B579A"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF2B579A"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1">
-      <alignment horizontal="center" vertical="center"/>
+  <cellStyleXfs count="22">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="ConditionalFormatStyle" xfId="1"/>
-    <cellStyle name="HeaderStyle" xfId="2"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="ConditionalFormatStyle" xfId="20"/>
+    <cellStyle name="HeaderStyle" xfId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFE7E7E7"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF2B579A"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4285f4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ea4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="fbbc04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="34a853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="ff6d01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="46bdc6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -365,34 +485,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -405,13 +515,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -421,15 +525,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -437,7 +539,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -445,12 +546,11 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -459,37 +559,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryRight="0" summaryBelow="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="L1">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="23.57031" customWidth="1"/>
-    <col min="3" max="3" width="43.92969" customWidth="1"/>
-    <col min="4" max="4" width="20.17969" customWidth="1"/>
-    <col min="5" max="5" width="18.57031" customWidth="1"/>
-    <col min="6" max="6" width="18.39063" customWidth="1"/>
-    <col min="7" max="7" width="16.77734" customWidth="1"/>
-    <col min="8" max="9" width="19.09766" customWidth="1"/>
-    <col min="10" max="10" width="20.17969" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.70703" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.59766" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.52734" customWidth="1"/>
-    <col min="14" max="14" width="15.17969" customWidth="1"/>
-    <col min="15" max="17" width="19.09766" customWidth="1"/>
-    <col min="18" max="18" width="29.45703" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="18.92969" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="29.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.93"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -507,13 +608,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -525,36 +626,36 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="33.75" customHeight="1">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -563,19 +664,19 @@
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -611,12 +712,12 @@
       <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -625,19 +726,19 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -670,15 +771,15 @@
       <c r="R3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -687,19 +788,19 @@
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -732,15 +833,15 @@
       <c r="R4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -749,19 +850,19 @@
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -794,15 +895,15 @@
       <c r="R5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -811,19 +912,19 @@
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -859,12 +960,12 @@
       <c r="S6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -873,19 +974,19 @@
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -918,15 +1019,15 @@
       <c r="R7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -935,19 +1036,19 @@
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="3" t="n">
         <v>500</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -980,15 +1081,15 @@
       <c r="R8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -997,19 +1098,19 @@
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="3" t="n">
         <v>500</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1042,15 +1143,15 @@
       <c r="R9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1059,19 +1160,19 @@
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F10" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="3" t="n">
         <v>500</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1107,12 +1208,12 @@
       <c r="S10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1121,19 +1222,19 @@
       <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="F11" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="3" t="n">
         <v>500</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1169,12 +1270,12 @@
       <c r="S11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1183,19 +1284,19 @@
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="F12" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G12" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1228,15 +1329,15 @@
       <c r="R12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1245,19 +1346,19 @@
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="F13" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1290,15 +1391,15 @@
       <c r="R13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1307,19 +1408,19 @@
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1352,15 +1453,15 @@
       <c r="R14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1369,19 +1470,19 @@
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F15" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1417,12 +1518,12 @@
       <c r="S15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T15">
-        <v>5</v>
+      <c r="T15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1431,19 +1532,19 @@
       <c r="C16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="F16" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G16" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1483,8 +1584,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1493,19 +1594,19 @@
       <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="2" t="n">
         <v>123456</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="F17" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G17" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="1" t="n">
         <v>500</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -1541,11 +1642,17 @@
       <c r="S17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="0" t="n">
         <v>600</v>
       </c>
     </row>
   </sheetData>
-  <headerFooter alignWithMargins="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>